<commit_message>
RunTableAdditions.xlsx file is updated. 1) The reagon with a changed slit position is marked. \n 2) the sum of charge*l_target/8. was calculated for the changed slit period
</commit_message>
<xml_diff>
--- a/RunTableAdditions.xlsx
+++ b/RunTableAdditions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="269">
   <si>
     <t xml:space="preserve">number</t>
   </si>
@@ -801,28 +801,6 @@
 Nothing in Goofle spreadsheet</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">No entry in google spreadsheet for this run
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No log entries for this run</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">No entry in google spreadsheet for this run
 No log entries for this run</t>
   </si>
@@ -833,26 +811,8 @@
     <t xml:space="preserve">Google spreadsheet tells “Junk”</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">test
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Google spreadsheet tells “Junk/test”</t>
-    </r>
+    <t xml:space="preserve">test
+Google spreadsheet tells “Junk/test”</t>
   </si>
   <si>
     <t xml:space="preserve">Google spreadsheet tells “Junk/test”</t>
@@ -913,16 +873,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">No entry in google spreadsheet for this run
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No log entries for this run
+No log entries for this run
 In the shift summary:
  DAQ alarm, rates drop to 0, we are ending run
  And restarting it. End run failed.
@@ -935,6 +886,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">I think it is worth to keep this run</t>
     </r>
@@ -946,54 +898,18 @@
 Think data might be useful</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">production
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No entry in the Google spreadsheet, but from
+    <t xml:space="preserve">production
+No entry in the Google spreadsheet, but from
 Logbook, seems DAQ crashed after about
 10-15 or more minutes after the start. So I
 Think data might be useful</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">No entry in google spreadsheet for this run
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The comment in shift summary is: 
+  </si>
+  <si>
+    <t xml:space="preserve">No entry in google spreadsheet for this run
+The comment in shift summary is: 
 ”08:37 - Livetime 80% upon starting 10485, 
 Retrying ...”
 This is 1 min run</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">No entry in google spreadsheet for this run.
@@ -1055,7 +971,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1095,12 +1011,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <u val="single"/>
       <sz val="11"/>
@@ -1115,14 +1025,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87D1D1"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1178,7 +1095,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1191,7 +1108,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1199,7 +1128,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1207,7 +1136,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1258,7 +1187,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF87D1D1"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFDB94D"/>
@@ -1290,8 +1219,8 @@
   </sheetPr>
   <dimension ref="A1:L412"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A384" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A411" activeCellId="1" sqref="L18 A411"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A231" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A249" activeCellId="0" sqref="249:289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1301,7 +1230,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.53"/>
@@ -10150,1515 +10079,1515 @@
         <v>140</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="n">
+    <row r="249" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="3" t="n">
         <v>10463</v>
       </c>
-      <c r="B249" s="2" t="n">
+      <c r="B249" s="4" t="n">
         <v>43701.8477662037</v>
       </c>
-      <c r="C249" s="2" t="n">
+      <c r="C249" s="4" t="n">
         <v>43701.8556828704</v>
       </c>
-      <c r="D249" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E249" s="0" t="s">
+      <c r="D249" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E249" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F249" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G249" s="0" t="n">
+      <c r="F249" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G249" s="5" t="n">
         <v>11539139</v>
       </c>
-      <c r="H249" s="0" t="n">
+      <c r="H249" s="5" t="n">
         <v>25183842753</v>
       </c>
-      <c r="I249" s="0" t="n">
+      <c r="I249" s="5" t="n">
         <v>0.0442569562327692</v>
       </c>
-      <c r="J249" s="0" t="n">
+      <c r="J249" s="5" t="n">
         <v>147.019631841557</v>
       </c>
-      <c r="K249" s="0" t="s">
+      <c r="K249" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1" t="n">
+    <row r="250" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="3" t="n">
         <v>10464</v>
       </c>
-      <c r="B250" s="2" t="n">
+      <c r="B250" s="4" t="n">
         <v>43701.8598958333</v>
       </c>
-      <c r="C250" s="2" t="n">
+      <c r="C250" s="4" t="n">
         <v>43701.8714583333</v>
       </c>
-      <c r="D250" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E250" s="0" t="s">
+      <c r="D250" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E250" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F250" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G250" s="0" t="n">
+      <c r="F250" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G250" s="5" t="n">
         <v>22030523</v>
       </c>
-      <c r="H250" s="0" t="n">
+      <c r="H250" s="5" t="n">
         <v>25205873276</v>
       </c>
-      <c r="I250" s="0" t="n">
+      <c r="I250" s="5" t="n">
         <v>0.0762995655488763</v>
       </c>
-      <c r="J250" s="0" t="n">
+      <c r="J250" s="5" t="n">
         <v>147.095931407106</v>
       </c>
-      <c r="K250" s="0" t="s">
+      <c r="K250" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1" t="n">
+    <row r="251" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="3" t="n">
         <v>10465</v>
       </c>
-      <c r="B251" s="2" t="n">
+      <c r="B251" s="4" t="n">
         <v>43701.8820949074</v>
       </c>
-      <c r="C251" s="2" t="n">
+      <c r="C251" s="4" t="n">
         <v>43701.992650463</v>
       </c>
-      <c r="D251" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E251" s="0" t="s">
+      <c r="D251" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E251" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F251" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G251" s="0" t="n">
+      <c r="F251" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G251" s="5" t="n">
         <v>229826627</v>
       </c>
-      <c r="H251" s="0" t="n">
+      <c r="H251" s="5" t="n">
         <v>25435699903</v>
       </c>
-      <c r="I251" s="0" t="n">
+      <c r="I251" s="5" t="n">
         <v>0.791950000762741</v>
       </c>
-      <c r="J251" s="0" t="n">
+      <c r="J251" s="5" t="n">
         <v>147.887881407868</v>
       </c>
-      <c r="K251" s="0" t="s">
+      <c r="K251" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L251" s="0" t="s">
+      <c r="L251" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="n">
+    <row r="252" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="3" t="n">
         <v>10479</v>
       </c>
-      <c r="B252" s="2" t="n">
+      <c r="B252" s="4" t="n">
         <v>43702.0901273148</v>
       </c>
-      <c r="C252" s="2" t="n">
+      <c r="C252" s="4" t="n">
         <v>43702.1132523148</v>
       </c>
-      <c r="D252" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E252" s="0" t="s">
+      <c r="D252" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E252" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F252" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G252" s="0" t="n">
+      <c r="F252" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G252" s="5" t="n">
         <v>41760846</v>
       </c>
-      <c r="H252" s="0" t="n">
+      <c r="H252" s="5" t="n">
         <v>25477460749</v>
       </c>
-      <c r="I252" s="0" t="n">
+      <c r="I252" s="5" t="n">
         <v>0.146155059850228</v>
       </c>
-      <c r="J252" s="0" t="n">
+      <c r="J252" s="5" t="n">
         <v>148.034036467719</v>
       </c>
-      <c r="K252" s="0" t="s">
+      <c r="K252" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="1" t="n">
+    <row r="253" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="3" t="n">
         <v>10480</v>
       </c>
-      <c r="B253" s="2" t="n">
+      <c r="B253" s="4" t="n">
         <v>43702.1175694444</v>
       </c>
-      <c r="C253" s="2" t="n">
+      <c r="C253" s="4" t="n">
         <v>43702.2233564815</v>
       </c>
-      <c r="D253" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E253" s="0" t="s">
+      <c r="D253" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E253" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F253" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G253" s="0" t="n">
+      <c r="F253" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G253" s="5" t="n">
         <v>210014424</v>
       </c>
-      <c r="H253" s="0" t="n">
+      <c r="H253" s="5" t="n">
         <v>25687475173</v>
       </c>
-      <c r="I253" s="0" t="n">
+      <c r="I253" s="5" t="n">
         <v>0.736578467540013</v>
       </c>
-      <c r="J253" s="0" t="n">
+      <c r="J253" s="5" t="n">
         <v>148.770614935259</v>
       </c>
-      <c r="K253" s="0" t="s">
+      <c r="K253" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="1" t="n">
+    <row r="254" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="3" t="n">
         <v>10484</v>
       </c>
-      <c r="B254" s="2" t="n">
+      <c r="B254" s="4" t="n">
         <v>43702.2664930556</v>
       </c>
-      <c r="C254" s="2" t="n">
+      <c r="C254" s="4" t="n">
         <v>43702.34125</v>
       </c>
-      <c r="D254" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E254" s="0" t="s">
+      <c r="D254" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E254" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F254" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G254" s="0" t="n">
+      <c r="F254" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G254" s="5" t="n">
         <v>145868295</v>
       </c>
-      <c r="H254" s="0" t="n">
+      <c r="H254" s="5" t="n">
         <v>25833343468</v>
       </c>
-      <c r="I254" s="0" t="n">
+      <c r="I254" s="5" t="n">
         <v>0.502762286540648</v>
       </c>
-      <c r="J254" s="0" t="n">
+      <c r="J254" s="5" t="n">
         <v>149.273377221799</v>
       </c>
-      <c r="K254" s="0" t="s">
+      <c r="K254" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="1" t="n">
+    <row r="255" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="3" t="n">
         <v>10485</v>
       </c>
-      <c r="B255" s="2" t="n">
+      <c r="B255" s="4" t="n">
         <v>43702.3639699074</v>
       </c>
-      <c r="C255" s="2" t="n">
+      <c r="C255" s="4" t="n">
         <v>43702.365</v>
       </c>
-      <c r="D255" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E255" s="0" t="s">
+      <c r="D255" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E255" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F255" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G255" s="0" t="n">
+      <c r="F255" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G255" s="5" t="n">
         <v>1646586</v>
       </c>
-      <c r="H255" s="0" t="n">
+      <c r="H255" s="5" t="n">
         <v>25834990054</v>
       </c>
-      <c r="I255" s="0" t="n">
+      <c r="I255" s="5" t="n">
         <v>0.00627976754987283</v>
       </c>
-      <c r="J255" s="0" t="n">
+      <c r="J255" s="5" t="n">
         <v>149.279656989349</v>
       </c>
-      <c r="K255" s="0" t="s">
+      <c r="K255" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="1" t="n">
+    <row r="256" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="3" t="n">
         <v>10486</v>
       </c>
-      <c r="B256" s="2" t="n">
+      <c r="B256" s="4" t="n">
         <v>43702.3665162037</v>
       </c>
-      <c r="C256" s="2" t="n">
+      <c r="C256" s="4" t="n">
         <v>43702.3949074074</v>
       </c>
-      <c r="D256" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E256" s="0" t="s">
+      <c r="D256" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E256" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F256" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G256" s="0" t="n">
+      <c r="F256" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G256" s="5" t="n">
         <v>41394805</v>
       </c>
-      <c r="H256" s="0" t="n">
+      <c r="H256" s="5" t="n">
         <v>25876384859</v>
       </c>
-      <c r="I256" s="0" t="n">
+      <c r="I256" s="5" t="n">
         <v>0.146914634255567</v>
       </c>
-      <c r="J256" s="0" t="n">
+      <c r="J256" s="5" t="n">
         <v>149.426571623605</v>
       </c>
-      <c r="K256" s="0" t="s">
+      <c r="K256" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="1" t="n">
+    <row r="257" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="3" t="n">
         <v>10487</v>
       </c>
-      <c r="B257" s="2" t="n">
+      <c r="B257" s="4" t="n">
         <v>43702.4357523148</v>
       </c>
-      <c r="C257" s="2" t="n">
+      <c r="C257" s="4" t="n">
         <v>43702.5930555556</v>
       </c>
-      <c r="D257" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E257" s="0" t="s">
+      <c r="D257" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E257" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F257" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G257" s="0" t="n">
+      <c r="F257" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G257" s="5" t="n">
         <v>310531365</v>
       </c>
-      <c r="H257" s="0" t="n">
+      <c r="H257" s="5" t="n">
         <v>26186916224</v>
       </c>
-      <c r="I257" s="0" t="n">
+      <c r="I257" s="5" t="n">
         <v>1.06686640486657</v>
       </c>
-      <c r="J257" s="0" t="n">
+      <c r="J257" s="5" t="n">
         <v>150.493438028471</v>
       </c>
-      <c r="K257" s="0" t="s">
+      <c r="K257" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="1" t="n">
+    <row r="258" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="3" t="n">
         <v>10491</v>
       </c>
-      <c r="B258" s="2" t="n">
+      <c r="B258" s="4" t="n">
         <v>43702.611712963</v>
       </c>
-      <c r="C258" s="2" t="n">
+      <c r="C258" s="4" t="n">
         <v>43702.6150810185</v>
       </c>
-      <c r="D258" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E258" s="0" t="s">
+      <c r="D258" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E258" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F258" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G258" s="0" t="n">
+      <c r="F258" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G258" s="5" t="n">
         <v>7410777</v>
       </c>
-      <c r="H258" s="0" t="n">
+      <c r="H258" s="5" t="n">
         <v>26194327001</v>
       </c>
-      <c r="I258" s="0" t="n">
+      <c r="I258" s="5" t="n">
         <v>0.0248719375924678</v>
       </c>
-      <c r="J258" s="0" t="n">
+      <c r="J258" s="5" t="n">
         <v>150.518309966064</v>
       </c>
-      <c r="K258" s="0" t="s">
+      <c r="K258" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="L258" s="0" t="s">
+      <c r="L258" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="1" t="n">
+    <row r="259" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="3" t="n">
         <v>10492</v>
       </c>
-      <c r="B259" s="2" t="n">
+      <c r="B259" s="4" t="n">
         <v>43702.6171527778</v>
       </c>
-      <c r="C259" s="2" t="n">
+      <c r="C259" s="4" t="n">
         <v>43702.6252430556</v>
       </c>
-      <c r="D259" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E259" s="0" t="s">
+      <c r="D259" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E259" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F259" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G259" s="0" t="n">
+      <c r="F259" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G259" s="5" t="n">
         <v>16152787</v>
       </c>
-      <c r="H259" s="0" t="n">
+      <c r="H259" s="5" t="n">
         <v>26210479788</v>
       </c>
-      <c r="I259" s="0" t="n">
+      <c r="I259" s="5" t="n">
         <v>0.0547109004011388</v>
       </c>
-      <c r="J259" s="0" t="n">
+      <c r="J259" s="5" t="n">
         <v>150.573020866465</v>
       </c>
-      <c r="K259" s="0" t="s">
+      <c r="K259" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="L259" s="0" t="s">
+      <c r="L259" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="1" t="n">
+    <row r="260" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="3" t="n">
         <v>10494</v>
       </c>
-      <c r="B260" s="2" t="n">
+      <c r="B260" s="4" t="n">
         <v>43702.6316203704</v>
       </c>
-      <c r="C260" s="2" t="n">
+      <c r="C260" s="4" t="n">
         <v>43702.6526967593</v>
       </c>
-      <c r="D260" s="0" t="s">
+      <c r="D260" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E260" s="0" t="s">
+      <c r="E260" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F260" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G260" s="0" t="n">
+      <c r="F260" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G260" s="5" t="n">
         <v>7494691</v>
       </c>
-      <c r="I260" s="0" t="n">
+      <c r="I260" s="5" t="n">
         <v>0.0836692141054876</v>
       </c>
-      <c r="K260" s="0" t="s">
+      <c r="K260" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L260" s="0" t="s">
+      <c r="L260" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="1" t="n">
+    <row r="261" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="3" t="n">
         <v>10495</v>
       </c>
-      <c r="B261" s="2" t="n">
+      <c r="B261" s="4" t="n">
         <v>43702.6548611111</v>
       </c>
-      <c r="C261" s="2" t="n">
+      <c r="C261" s="4" t="n">
         <v>43702.7035300926</v>
       </c>
-      <c r="D261" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E261" s="0" t="s">
+      <c r="D261" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E261" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F261" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G261" s="0" t="n">
+      <c r="F261" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G261" s="5" t="n">
         <v>100442091</v>
       </c>
-      <c r="H261" s="0" t="n">
+      <c r="H261" s="5" t="n">
         <v>26310921879</v>
       </c>
-      <c r="I261" s="0" t="n">
+      <c r="I261" s="5" t="n">
         <v>0.341327023391157</v>
       </c>
-      <c r="J261" s="0" t="n">
+      <c r="J261" s="5" t="n">
         <v>150.914347889856</v>
       </c>
-      <c r="K261" s="0" t="s">
+      <c r="K261" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L261" s="0" t="s">
+      <c r="L261" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="1" t="n">
+    <row r="262" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="3" t="n">
         <v>10496</v>
       </c>
-      <c r="B262" s="2" t="n">
+      <c r="B262" s="4" t="n">
         <v>43702.7092013889</v>
       </c>
-      <c r="C262" s="2" t="n">
+      <c r="C262" s="4" t="n">
         <v>43702.7778819444</v>
       </c>
-      <c r="D262" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E262" s="0" t="s">
+      <c r="D262" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E262" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F262" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G262" s="0" t="n">
+      <c r="F262" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G262" s="5" t="n">
         <v>152795545</v>
       </c>
-      <c r="H262" s="0" t="n">
+      <c r="H262" s="5" t="n">
         <v>26463717424</v>
       </c>
-      <c r="I262" s="0" t="n">
+      <c r="I262" s="5" t="n">
         <v>0.519439894920425</v>
       </c>
-      <c r="J262" s="0" t="n">
+      <c r="J262" s="5" t="n">
         <v>151.433787784776</v>
       </c>
-      <c r="K262" s="0" t="s">
+      <c r="K262" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L262" s="0" t="s">
+      <c r="L262" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="1" t="n">
+    <row r="263" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="3" t="n">
         <v>10498</v>
       </c>
-      <c r="B263" s="2" t="n">
+      <c r="B263" s="4" t="n">
         <v>43702.8015046296</v>
       </c>
-      <c r="C263" s="2" t="n">
+      <c r="C263" s="4" t="n">
         <v>43702.9478587963</v>
       </c>
-      <c r="D263" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E263" s="0" t="s">
+      <c r="D263" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E263" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F263" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G263" s="0" t="n">
+      <c r="F263" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G263" s="5" t="n">
         <v>310490534</v>
       </c>
-      <c r="H263" s="0" t="n">
+      <c r="H263" s="5" t="n">
         <v>26774207958</v>
       </c>
-      <c r="I263" s="0" t="n">
+      <c r="I263" s="5" t="n">
         <v>1.06928107126345</v>
       </c>
-      <c r="J263" s="0" t="n">
+      <c r="J263" s="5" t="n">
         <v>152.50306885604</v>
       </c>
-      <c r="K263" s="0" t="s">
+      <c r="K263" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L263" s="0" t="s">
+      <c r="L263" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1" t="n">
+    <row r="264" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="3" t="n">
         <v>10499</v>
       </c>
-      <c r="B264" s="2" t="n">
+      <c r="B264" s="4" t="n">
         <v>43702.9635300926</v>
       </c>
-      <c r="C264" s="2" t="n">
+      <c r="C264" s="4" t="n">
         <v>43702.9676041667</v>
       </c>
-      <c r="D264" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E264" s="0" t="s">
+      <c r="D264" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E264" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F264" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G264" s="0" t="n">
+      <c r="F264" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G264" s="5" t="n">
         <v>8436367</v>
       </c>
-      <c r="H264" s="0" t="n">
+      <c r="H264" s="5" t="n">
         <v>26782644325</v>
       </c>
-      <c r="I264" s="0" t="n">
+      <c r="I264" s="5" t="n">
         <v>0.0284962685151097</v>
       </c>
-      <c r="J264" s="0" t="n">
+      <c r="J264" s="5" t="n">
         <v>152.531565124555</v>
       </c>
-      <c r="K264" s="0" t="s">
+      <c r="K264" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="n">
+    <row r="265" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="3" t="n">
         <v>10502</v>
       </c>
-      <c r="B265" s="2" t="n">
+      <c r="B265" s="4" t="n">
         <v>43702.9856828704</v>
       </c>
-      <c r="C265" s="2" t="n">
+      <c r="C265" s="4" t="n">
         <v>43703.1289467593</v>
       </c>
-      <c r="D265" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E265" s="0" t="s">
+      <c r="D265" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E265" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F265" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G265" s="0" t="n">
+      <c r="F265" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G265" s="5" t="n">
         <v>300951448</v>
       </c>
-      <c r="H265" s="0" t="n">
+      <c r="H265" s="5" t="n">
         <v>27083595773</v>
       </c>
-      <c r="I265" s="0" t="n">
+      <c r="I265" s="5" t="n">
         <v>1.02666444594638</v>
       </c>
-      <c r="J265" s="0" t="n">
+      <c r="J265" s="5" t="n">
         <v>153.558229570501</v>
       </c>
-      <c r="K265" s="0" t="s">
+      <c r="K265" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="1" t="n">
+    <row r="266" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="3" t="n">
         <v>10503</v>
       </c>
-      <c r="B266" s="2" t="n">
+      <c r="B266" s="4" t="n">
         <v>43703.1440740741</v>
       </c>
-      <c r="C266" s="2" t="n">
+      <c r="C266" s="4" t="n">
         <v>43703.2708680556</v>
       </c>
-      <c r="D266" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E266" s="0" t="s">
+      <c r="D266" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E266" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F266" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G266" s="0" t="n">
+      <c r="F266" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G266" s="5" t="n">
         <v>291288772</v>
       </c>
-      <c r="H266" s="0" t="n">
+      <c r="H266" s="5" t="n">
         <v>27374884545</v>
       </c>
-      <c r="I266" s="0" t="n">
+      <c r="I266" s="5" t="n">
         <v>0.991456895194432</v>
       </c>
-      <c r="J266" s="0" t="n">
+      <c r="J266" s="5" t="n">
         <v>154.549686465696</v>
       </c>
-      <c r="K266" s="0" t="s">
+      <c r="K266" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="1" t="n">
+    <row r="267" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="3" t="n">
         <v>10505</v>
       </c>
-      <c r="B267" s="2" t="n">
+      <c r="B267" s="4" t="n">
         <v>43703.306087963</v>
       </c>
-      <c r="C267" s="2" t="n">
+      <c r="C267" s="4" t="n">
         <v>43703.3396296296</v>
       </c>
-      <c r="D267" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E267" s="0" t="s">
+      <c r="D267" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E267" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F267" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G267" s="0" t="n">
+      <c r="F267" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G267" s="5" t="n">
         <v>67545184</v>
       </c>
-      <c r="H267" s="0" t="n">
+      <c r="H267" s="5" t="n">
         <v>27442429729</v>
       </c>
-      <c r="I267" s="0" t="n">
+      <c r="I267" s="5" t="n">
         <v>0.231755506338351</v>
       </c>
-      <c r="J267" s="0" t="n">
+      <c r="J267" s="5" t="n">
         <v>154.781441972034</v>
       </c>
-      <c r="K267" s="0" t="s">
+      <c r="K267" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="1" t="n">
+    <row r="268" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="3" t="n">
         <v>10508</v>
       </c>
-      <c r="B268" s="2" t="n">
+      <c r="B268" s="4" t="n">
         <v>43703.3656134259</v>
       </c>
-      <c r="C268" s="2" t="n">
+      <c r="C268" s="4" t="n">
         <v>43703.3806712963</v>
       </c>
-      <c r="D268" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E268" s="0" t="s">
+      <c r="D268" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E268" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F268" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G268" s="0" t="n">
+      <c r="F268" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G268" s="5" t="n">
         <v>34063440</v>
       </c>
-      <c r="H268" s="0" t="n">
+      <c r="H268" s="5" t="n">
         <v>27476493169</v>
       </c>
-      <c r="I268" s="0" t="n">
+      <c r="I268" s="5" t="n">
         <v>0.112996008799069</v>
       </c>
-      <c r="J268" s="0" t="n">
+      <c r="J268" s="5" t="n">
         <v>154.894437980833</v>
       </c>
-      <c r="K268" s="0" t="s">
+      <c r="K268" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="1" t="n">
+    <row r="269" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="3" t="n">
         <v>10509</v>
       </c>
-      <c r="B269" s="2" t="n">
+      <c r="B269" s="4" t="n">
         <v>43703.383587963</v>
       </c>
-      <c r="C269" s="2" t="n">
+      <c r="C269" s="4" t="n">
         <v>43703.3913657407</v>
       </c>
-      <c r="D269" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E269" s="0" t="s">
+      <c r="D269" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E269" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F269" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G269" s="0" t="n">
+      <c r="F269" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G269" s="5" t="n">
         <v>16188233</v>
       </c>
-      <c r="H269" s="0" t="n">
+      <c r="H269" s="5" t="n">
         <v>27492681402</v>
       </c>
-      <c r="I269" s="0" t="n">
+      <c r="I269" s="5" t="n">
         <v>0.0538458014776641</v>
       </c>
-      <c r="J269" s="0" t="n">
+      <c r="J269" s="5" t="n">
         <v>154.948283782311</v>
       </c>
-      <c r="K269" s="0" t="s">
+      <c r="K269" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="1" t="n">
+    <row r="270" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="3" t="n">
         <v>10512</v>
       </c>
-      <c r="B270" s="2" t="n">
+      <c r="B270" s="4" t="n">
         <v>43703.4141319445</v>
       </c>
-      <c r="C270" s="2" t="n">
+      <c r="C270" s="4" t="n">
         <v>43703.441875</v>
       </c>
-      <c r="D270" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E270" s="0" t="s">
+      <c r="D270" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E270" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F270" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G270" s="0" t="n">
+      <c r="F270" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G270" s="5" t="n">
         <v>53660189</v>
       </c>
-      <c r="H270" s="0" t="n">
+      <c r="H270" s="5" t="n">
         <v>27546341591</v>
       </c>
-      <c r="I270" s="0" t="n">
+      <c r="I270" s="5" t="n">
         <v>0.188264307041074</v>
       </c>
-      <c r="J270" s="0" t="n">
+      <c r="J270" s="5" t="n">
         <v>155.136548089352</v>
       </c>
-      <c r="K270" s="0" t="s">
+      <c r="K270" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="1" t="n">
+    <row r="271" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="3" t="n">
         <v>10514</v>
       </c>
-      <c r="B271" s="2" t="n">
+      <c r="B271" s="4" t="n">
         <v>43703.4589351852</v>
       </c>
-      <c r="C271" s="2" t="n">
+      <c r="C271" s="4" t="n">
         <v>43703.5836805556</v>
       </c>
-      <c r="D271" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E271" s="0" t="s">
+      <c r="D271" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E271" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F271" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G271" s="0" t="n">
+      <c r="F271" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G271" s="5" t="n">
         <v>250570948</v>
       </c>
-      <c r="H271" s="0" t="n">
+      <c r="H271" s="5" t="n">
         <v>27796912539</v>
       </c>
-      <c r="I271" s="0" t="n">
+      <c r="I271" s="5" t="n">
         <v>0.876955232284512</v>
       </c>
-      <c r="J271" s="0" t="n">
+      <c r="J271" s="5" t="n">
         <v>156.013503321636</v>
       </c>
-      <c r="K271" s="0" t="s">
+      <c r="K271" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="1" t="n">
+    <row r="272" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="3" t="n">
         <v>10515</v>
       </c>
-      <c r="B272" s="2" t="n">
+      <c r="B272" s="4" t="n">
         <v>43703.7353703704</v>
       </c>
-      <c r="C272" s="2" t="n">
+      <c r="C272" s="4" t="n">
         <v>43703.7430439815</v>
       </c>
-      <c r="D272" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E272" s="0" t="s">
+      <c r="D272" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E272" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F272" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G272" s="0" t="n">
+      <c r="F272" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G272" s="5" t="n">
         <v>12133592</v>
       </c>
-      <c r="H272" s="0" t="n">
+      <c r="H272" s="5" t="n">
         <v>27809046131</v>
       </c>
-      <c r="I272" s="0" t="n">
+      <c r="I272" s="5" t="n">
         <v>0.127054024043081</v>
       </c>
-      <c r="J272" s="0" t="n">
+      <c r="J272" s="5" t="n">
         <v>156.140557345679</v>
       </c>
-      <c r="K272" s="0" t="s">
+      <c r="K272" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="1" t="n">
+    <row r="273" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="3" t="n">
         <v>10516</v>
       </c>
-      <c r="B273" s="2" t="n">
+      <c r="B273" s="4" t="n">
         <v>43703.7529861111</v>
       </c>
-      <c r="C273" s="2" t="n">
+      <c r="C273" s="4" t="n">
         <v>43703.7548263889</v>
       </c>
-      <c r="D273" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E273" s="0" t="s">
+      <c r="D273" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E273" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F273" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G273" s="0" t="n">
+      <c r="F273" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G273" s="5" t="n">
         <v>3664418</v>
       </c>
-      <c r="H273" s="0" t="n">
+      <c r="H273" s="5" t="n">
         <v>27812710549</v>
       </c>
-      <c r="I273" s="0" t="n">
+      <c r="I273" s="5" t="n">
         <v>0.0374564818236512</v>
       </c>
-      <c r="J273" s="0" t="n">
+      <c r="J273" s="5" t="n">
         <v>156.178013827503</v>
       </c>
-      <c r="K273" s="0" t="s">
+      <c r="K273" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="n">
+    <row r="274" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="3" t="n">
         <v>10517</v>
       </c>
-      <c r="B274" s="2" t="n">
+      <c r="B274" s="4" t="n">
         <v>43703.7702083333</v>
       </c>
-      <c r="C274" s="2" t="n">
+      <c r="C274" s="4" t="n">
         <v>43703.7815162037</v>
       </c>
-      <c r="D274" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E274" s="0" t="s">
+      <c r="D274" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E274" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F274" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G274" s="0" t="n">
+      <c r="F274" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G274" s="5" t="n">
         <v>23451576</v>
       </c>
-      <c r="H274" s="0" t="n">
+      <c r="H274" s="5" t="n">
         <v>27836162125</v>
       </c>
-      <c r="I274" s="0" t="n">
+      <c r="I274" s="5" t="n">
         <v>0.235311846746109</v>
       </c>
-      <c r="J274" s="0" t="n">
+      <c r="J274" s="5" t="n">
         <v>156.413325674249</v>
       </c>
-      <c r="K274" s="0" t="s">
+      <c r="K274" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="1" t="n">
+    <row r="275" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="3" t="n">
         <v>10518</v>
       </c>
-      <c r="B275" s="2" t="n">
+      <c r="B275" s="4" t="n">
         <v>43703.7835532407</v>
       </c>
-      <c r="C275" s="2" t="n">
+      <c r="C275" s="4" t="n">
         <v>43703.9365740741</v>
       </c>
-      <c r="D275" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E275" s="0" t="s">
+      <c r="D275" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E275" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F275" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G275" s="0" t="n">
+      <c r="F275" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G275" s="5" t="n">
         <v>314117775</v>
       </c>
-      <c r="H275" s="0" t="n">
+      <c r="H275" s="5" t="n">
         <v>28150279900</v>
       </c>
-      <c r="I275" s="0" t="n">
+      <c r="I275" s="5" t="n">
         <v>3.16619443608224</v>
       </c>
-      <c r="J275" s="0" t="n">
+      <c r="J275" s="5" t="n">
         <v>159.579520110332</v>
       </c>
-      <c r="K275" s="0" t="s">
+      <c r="K275" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="L275" s="0" t="s">
+      <c r="L275" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1" t="n">
+    <row r="276" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="3" t="n">
         <v>10519</v>
       </c>
-      <c r="B276" s="2" t="n">
+      <c r="B276" s="4" t="n">
         <v>43703.941412037</v>
       </c>
-      <c r="C276" s="2" t="n">
+      <c r="C276" s="4" t="n">
         <v>43704.0450231481</v>
       </c>
-      <c r="D276" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E276" s="0" t="s">
+      <c r="D276" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E276" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F276" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G276" s="0" t="n">
+      <c r="F276" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G276" s="5" t="n">
         <v>224304862</v>
       </c>
-      <c r="H276" s="0" t="n">
+      <c r="H276" s="5" t="n">
         <v>28374584762</v>
       </c>
-      <c r="I276" s="0" t="n">
+      <c r="I276" s="5" t="n">
         <v>2.25365322815924</v>
       </c>
-      <c r="J276" s="0" t="n">
+      <c r="J276" s="5" t="n">
         <v>161.833173338491</v>
       </c>
-      <c r="K276" s="0" t="s">
+      <c r="K276" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="L276" s="0" t="s">
+      <c r="L276" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="1" t="n">
+    <row r="277" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="3" t="n">
         <v>10520</v>
       </c>
-      <c r="B277" s="2" t="n">
+      <c r="B277" s="4" t="n">
         <v>43704.0568865741</v>
       </c>
-      <c r="C277" s="2" t="n">
+      <c r="C277" s="4" t="n">
         <v>43704.1607638889</v>
       </c>
-      <c r="D277" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E277" s="0" t="s">
+      <c r="D277" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E277" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F277" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G277" s="0" t="n">
+      <c r="F277" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G277" s="5" t="n">
         <v>224483711</v>
       </c>
-      <c r="H277" s="0" t="n">
+      <c r="H277" s="5" t="n">
         <v>28599068473</v>
       </c>
-      <c r="I277" s="0" t="n">
+      <c r="I277" s="5" t="n">
         <v>2.26160538744655</v>
       </c>
-      <c r="J277" s="0" t="n">
+      <c r="J277" s="5" t="n">
         <v>164.094778725937</v>
       </c>
-      <c r="K277" s="0" t="s">
+      <c r="K277" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="L277" s="0" t="s">
+      <c r="L277" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="1" t="n">
+    <row r="278" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="3" t="n">
         <v>10521</v>
       </c>
-      <c r="B278" s="2" t="n">
+      <c r="B278" s="4" t="n">
         <v>43704.1727893519</v>
       </c>
-      <c r="C278" s="2" t="n">
+      <c r="C278" s="4" t="n">
         <v>43704.2646990741</v>
       </c>
-      <c r="D278" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E278" s="0" t="s">
+      <c r="D278" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E278" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F278" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G278" s="0" t="n">
+      <c r="F278" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G278" s="5" t="n">
         <v>199954011</v>
       </c>
-      <c r="H278" s="0" t="n">
+      <c r="H278" s="5" t="n">
         <v>28799022484</v>
       </c>
-      <c r="I278" s="0" t="n">
+      <c r="I278" s="5" t="n">
         <v>1.99762561504544</v>
       </c>
-      <c r="J278" s="0" t="n">
+      <c r="J278" s="5" t="n">
         <v>166.092404340983</v>
       </c>
-      <c r="K278" s="0" t="s">
+      <c r="K278" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="L278" s="0" t="s">
+      <c r="L278" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="1" t="n">
+    <row r="279" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="3" t="n">
         <v>10522</v>
       </c>
-      <c r="B279" s="2" t="n">
+      <c r="B279" s="4" t="n">
         <v>43704.2798148148</v>
       </c>
-      <c r="C279" s="2" t="n">
+      <c r="C279" s="4" t="n">
         <v>43704.4000462963</v>
       </c>
-      <c r="D279" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E279" s="0" t="s">
+      <c r="D279" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E279" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F279" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G279" s="0" t="n">
+      <c r="F279" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G279" s="5" t="n">
         <v>247674517</v>
       </c>
-      <c r="H279" s="0" t="n">
+      <c r="H279" s="5" t="n">
         <v>29046697001</v>
       </c>
-      <c r="I279" s="0" t="n">
+      <c r="I279" s="5" t="n">
         <v>2.50989699997851</v>
       </c>
-      <c r="J279" s="0" t="n">
+      <c r="J279" s="5" t="n">
         <v>168.602301340961</v>
       </c>
-      <c r="K279" s="0" t="s">
+      <c r="K279" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="L279" s="0" t="s">
+      <c r="L279" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="1" t="n">
+    <row r="280" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="3" t="n">
         <v>10523</v>
       </c>
-      <c r="B280" s="2" t="n">
+      <c r="B280" s="4" t="n">
         <v>43704.4118634259</v>
       </c>
-      <c r="C280" s="2" t="n">
+      <c r="C280" s="4" t="n">
         <v>43704.4469675926</v>
       </c>
-      <c r="D280" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E280" s="0" t="s">
+      <c r="D280" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E280" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F280" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G280" s="0" t="n">
+      <c r="F280" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G280" s="5" t="n">
         <v>70507660</v>
       </c>
-      <c r="H280" s="0" t="n">
+      <c r="H280" s="5" t="n">
         <v>29117204661</v>
       </c>
-      <c r="I280" s="0" t="n">
+      <c r="I280" s="5" t="n">
         <v>0.243540696886248</v>
       </c>
-      <c r="J280" s="0" t="n">
+      <c r="J280" s="5" t="n">
         <v>168.845842037848</v>
       </c>
-      <c r="K280" s="0" t="s">
+      <c r="K280" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="L280" s="0" t="s">
+      <c r="L280" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="1" t="n">
+    <row r="281" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="3" t="n">
         <v>10524</v>
       </c>
-      <c r="B281" s="2" t="n">
+      <c r="B281" s="4" t="n">
         <v>43704.4540625</v>
       </c>
-      <c r="C281" s="2" t="n">
+      <c r="C281" s="4" t="n">
         <v>43704.6127430556</v>
       </c>
-      <c r="D281" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E281" s="0" t="s">
+      <c r="D281" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E281" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F281" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G281" s="0" t="n">
+      <c r="F281" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G281" s="5" t="n">
         <v>320269500</v>
       </c>
-      <c r="H281" s="0" t="n">
+      <c r="H281" s="5" t="n">
         <v>29437474161</v>
       </c>
-      <c r="I281" s="0" t="n">
+      <c r="I281" s="5" t="n">
         <v>1.13237491383758</v>
       </c>
-      <c r="J281" s="0" t="n">
+      <c r="J281" s="5" t="n">
         <v>169.978216951685</v>
       </c>
-      <c r="K281" s="0" t="s">
+      <c r="K281" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="L281" s="0" t="s">
+      <c r="L281" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="1" t="n">
+    <row r="282" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="3" t="n">
         <v>10525</v>
       </c>
-      <c r="B282" s="2" t="n">
+      <c r="B282" s="4" t="n">
         <v>43704.6794212963</v>
       </c>
-      <c r="C282" s="2" t="n">
+      <c r="C282" s="4" t="n">
         <v>43704.6842592593</v>
       </c>
-      <c r="D282" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E282" s="0" t="s">
+      <c r="D282" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E282" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F282" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G282" s="0" t="n">
+      <c r="F282" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G282" s="5" t="n">
         <v>7268303</v>
       </c>
-      <c r="H282" s="0" t="n">
+      <c r="H282" s="5" t="n">
         <v>29444742464</v>
       </c>
-      <c r="I282" s="0" t="n">
+      <c r="I282" s="5" t="n">
         <v>0.0780921946013622</v>
       </c>
-      <c r="J282" s="0" t="n">
+      <c r="J282" s="5" t="n">
         <v>170.056309146287</v>
       </c>
-      <c r="K282" s="0" t="s">
+      <c r="K282" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="L282" s="0" t="s">
+      <c r="L282" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="1" t="n">
+    <row r="283" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="3" t="n">
         <v>10526</v>
       </c>
-      <c r="B283" s="2" t="n">
+      <c r="B283" s="4" t="n">
         <v>43704.6946875</v>
       </c>
-      <c r="C283" s="2" t="n">
+      <c r="C283" s="4" t="n">
         <v>43704.872662037</v>
       </c>
-      <c r="D283" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E283" s="0" t="s">
+      <c r="D283" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E283" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F283" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G283" s="0" t="n">
+      <c r="F283" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G283" s="5" t="n">
         <v>254786189</v>
       </c>
-      <c r="H283" s="0" t="n">
+      <c r="H283" s="5" t="n">
         <v>29699528653</v>
       </c>
-      <c r="I283" s="0" t="n">
+      <c r="I283" s="5" t="n">
         <v>2.73488302972659</v>
       </c>
-      <c r="J283" s="0" t="n">
+      <c r="J283" s="5" t="n">
         <v>172.791192176013</v>
       </c>
-      <c r="K283" s="0" t="s">
+      <c r="K283" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="L283" s="0" t="s">
+      <c r="L283" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="1" t="n">
+    <row r="284" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="3" t="n">
         <v>10529</v>
       </c>
-      <c r="B284" s="2" t="n">
+      <c r="B284" s="4" t="n">
         <v>43704.8988773148</v>
       </c>
-      <c r="C284" s="2" t="n">
+      <c r="C284" s="4" t="n">
         <v>43705.0598958333</v>
       </c>
-      <c r="D284" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E284" s="0" t="s">
+      <c r="D284" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E284" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F284" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G284" s="0" t="n">
+      <c r="F284" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G284" s="5" t="n">
         <v>233466248</v>
       </c>
-      <c r="H284" s="0" t="n">
+      <c r="H284" s="5" t="n">
         <v>29932994901</v>
       </c>
-      <c r="I284" s="0" t="n">
+      <c r="I284" s="5" t="n">
         <v>2.48899540857389</v>
       </c>
-      <c r="J284" s="0" t="n">
+      <c r="J284" s="5" t="n">
         <v>175.280187584587</v>
       </c>
-      <c r="K284" s="0" t="s">
+      <c r="K284" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="L284" s="0" t="s">
+      <c r="L284" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="n">
+    <row r="285" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="3" t="n">
         <v>10530</v>
       </c>
-      <c r="B285" s="2" t="n">
+      <c r="B285" s="4" t="n">
         <v>43705.0751273148</v>
       </c>
-      <c r="C285" s="2" t="n">
+      <c r="C285" s="4" t="n">
         <v>43705.1157523148</v>
       </c>
-      <c r="D285" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E285" s="0" t="s">
+      <c r="D285" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E285" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F285" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G285" s="0" t="n">
+      <c r="F285" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G285" s="5" t="n">
         <v>60605300</v>
       </c>
-      <c r="H285" s="0" t="n">
+      <c r="H285" s="5" t="n">
         <v>29993600201</v>
       </c>
-      <c r="I285" s="0" t="n">
+      <c r="I285" s="5" t="n">
         <v>0.621647785445737</v>
       </c>
-      <c r="J285" s="0" t="n">
+      <c r="J285" s="5" t="n">
         <v>175.901835370033</v>
       </c>
-      <c r="K285" s="0" t="s">
+      <c r="K285" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="1" t="n">
+    <row r="286" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="3" t="n">
         <v>10531</v>
       </c>
-      <c r="B286" s="2" t="n">
+      <c r="B286" s="4" t="n">
         <v>43705.1210300926</v>
       </c>
-      <c r="C286" s="2" t="n">
+      <c r="C286" s="4" t="n">
         <v>43705.2684143518</v>
       </c>
-      <c r="D286" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E286" s="0" t="s">
+      <c r="D286" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E286" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F286" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G286" s="0" t="n">
+      <c r="F286" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G286" s="5" t="n">
         <v>217934967</v>
       </c>
-      <c r="H286" s="0" t="n">
+      <c r="H286" s="5" t="n">
         <v>30211535168</v>
       </c>
-      <c r="I286" s="0" t="n">
+      <c r="I286" s="5" t="n">
         <v>2.31100953881146</v>
       </c>
-      <c r="J286" s="0" t="n">
+      <c r="J286" s="5" t="n">
         <v>178.212844908844</v>
       </c>
-      <c r="K286" s="0" t="s">
+      <c r="K286" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="1" t="n">
+    <row r="287" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="3" t="n">
         <v>10532</v>
       </c>
-      <c r="B287" s="2" t="n">
+      <c r="B287" s="4" t="n">
         <v>43705.2785300926</v>
       </c>
-      <c r="C287" s="2" t="n">
+      <c r="C287" s="4" t="n">
         <v>43705.3656134259</v>
       </c>
-      <c r="D287" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E287" s="0" t="s">
+      <c r="D287" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E287" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F287" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G287" s="0" t="n">
+      <c r="F287" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G287" s="5" t="n">
         <v>128630247</v>
       </c>
-      <c r="H287" s="0" t="n">
+      <c r="H287" s="5" t="n">
         <v>30340165415</v>
       </c>
-      <c r="I287" s="0" t="n">
+      <c r="I287" s="5" t="n">
         <v>1.36420356984702</v>
       </c>
-      <c r="J287" s="0" t="n">
+      <c r="J287" s="5" t="n">
         <v>179.577048478691</v>
       </c>
-      <c r="K287" s="0" t="s">
+      <c r="K287" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="L287" s="0" t="s">
+      <c r="L287" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="n">
+    <row r="288" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="3" t="n">
         <v>10533</v>
       </c>
-      <c r="B288" s="2" t="n">
+      <c r="B288" s="4" t="n">
         <v>43705.3743865741</v>
       </c>
-      <c r="C288" s="2" t="n">
+      <c r="C288" s="4" t="n">
         <v>43705.3789236111</v>
       </c>
-      <c r="D288" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E288" s="0" t="s">
+      <c r="D288" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E288" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F288" s="0" t="n">
+      <c r="F288" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G288" s="0" t="n">
+      <c r="G288" s="5" t="n">
         <v>5313403</v>
       </c>
-      <c r="K288" s="0" t="s">
+      <c r="K288" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="L288" s="0" t="s">
+      <c r="L288" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="1" t="n">
+    <row r="289" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="3" t="n">
         <v>10534</v>
       </c>
-      <c r="B289" s="2" t="n">
+      <c r="B289" s="4" t="n">
         <v>43705.3927199074</v>
       </c>
-      <c r="C289" s="2" t="n">
+      <c r="C289" s="4" t="n">
         <v>43705.3970601852</v>
       </c>
-      <c r="D289" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E289" s="0" t="s">
+      <c r="D289" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E289" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F289" s="0" t="n">
+      <c r="F289" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G289" s="0" t="n">
+      <c r="G289" s="5" t="n">
         <v>5116256</v>
       </c>
-      <c r="K289" s="0" t="s">
+      <c r="K289" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="L289" s="0" t="s">
+      <c r="L289" s="5" t="s">
         <v>166</v>
       </c>
     </row>
@@ -16205,7 +16134,7 @@
   <dimension ref="A7:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="1" sqref="L18 L21"/>
+      <selection pane="topLeft" activeCell="L21" activeCellId="1" sqref="249:289 L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16221,7 +16150,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="7" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>10053</v>
       </c>
@@ -16231,27 +16160,27 @@
       <c r="C7" s="2" t="n">
         <v>43673.5590509259</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="n">
+      <c r="F7" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="7" t="n">
         <v>45324817</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="7" t="n">
         <v>0.362202748123273</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>10262</v>
       </c>
@@ -16261,27 +16190,27 @@
       <c r="C8" s="2" t="n">
         <v>43686.6612037037</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="n">
+      <c r="F8" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="7" t="n">
         <v>18463664</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="7" t="n">
         <v>0.131901663133459</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>10273</v>
       </c>
@@ -16291,23 +16220,23 @@
       <c r="C9" s="2" t="n">
         <v>43687.5902662037</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="n">
+      <c r="F9" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="7" t="n">
         <v>8250239</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I9" s="7" t="n">
         <v>0.0998378744923005</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -16315,14 +16244,14 @@
       <c r="A10" s="1" t="n">
         <v>10353</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10443</v>
       </c>
@@ -16332,23 +16261,23 @@
       <c r="C11" s="2" t="n">
         <v>43698.9361805556</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="7" t="n">
         <v>300014722</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="7" t="s">
         <v>139</v>
       </c>
     </row>
@@ -16356,7 +16285,7 @@
       <c r="A12" s="1" t="n">
         <v>10451</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -16364,11 +16293,11 @@
       <c r="A13" s="1" t="n">
         <v>10466</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>10494</v>
       </c>
@@ -16378,30 +16307,30 @@
       <c r="C14" s="2" t="n">
         <v>43702.6526967593</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="n">
+      <c r="F14" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="n">
         <v>7494691</v>
       </c>
-      <c r="I14" s="4" t="n">
+      <c r="I14" s="7" t="n">
         <v>0.0836692141054876</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>10533</v>
       </c>
@@ -16411,23 +16340,23 @@
       <c r="C15" s="2" t="n">
         <v>43705.3789236111</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="7" t="n">
         <v>5313403</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -16457,7 +16386,7 @@
       <c r="K16" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="6" t="s">
         <v>166</v>
       </c>
     </row>
@@ -16487,7 +16416,7 @@
       <c r="K17" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -16495,7 +16424,7 @@
       <c r="A18" s="1" t="n">
         <v>10581</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="6" t="s">
         <v>234</v>
       </c>
     </row>
@@ -16503,13 +16432,13 @@
       <c r="A19" s="1" t="n">
         <v>10640</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="6" t="s">
         <v>237</v>
       </c>
     </row>
@@ -16517,17 +16446,17 @@
       <c r="A20" s="1" t="n">
         <v>10696</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="21" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>10624</v>
       </c>
@@ -16537,32 +16466,32 @@
       <c r="C21" s="2" t="n">
         <v>43709.135162037</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G21" s="4" t="n">
+      <c r="F21" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="n">
         <v>2706956</v>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="7" t="n">
         <v>35868105017</v>
       </c>
-      <c r="I21" s="4" t="n">
+      <c r="I21" s="7" t="n">
         <v>0.0104652868707814</v>
       </c>
-      <c r="J21" s="4" t="n">
+      <c r="J21" s="7" t="n">
         <v>200.40309628621</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="6" t="s">
         <v>191</v>
       </c>
     </row>
@@ -16584,8 +16513,8 @@
   </sheetPr>
   <dimension ref="A14:L69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E80" activeCellId="1" sqref="L18 E80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="249:289 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16596,14 +16525,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="49.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="40.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="14" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>10055</v>
       </c>
@@ -16613,32 +16543,32 @@
       <c r="C14" s="2" t="n">
         <v>43673.692962963</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="n">
+      <c r="F14" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="n">
         <v>3371956</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="7" t="n">
         <v>1288976775</v>
       </c>
-      <c r="I14" s="4" t="n">
+      <c r="I14" s="7" t="n">
         <v>0.0309241202403067</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="7" t="n">
         <v>10.4295667850425</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -16677,7 +16607,7 @@
       <c r="K15" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -16716,11 +16646,11 @@
       <c r="K16" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>10061</v>
       </c>
@@ -16730,36 +16660,36 @@
       <c r="C17" s="2" t="n">
         <v>43673.7999305556</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="n">
+      <c r="F17" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="n">
         <v>4130186</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="7" t="n">
         <v>1305407048</v>
       </c>
-      <c r="I17" s="4" t="n">
+      <c r="I17" s="7" t="n">
         <v>0.0377328296685583</v>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="7" t="n">
         <v>10.6048095345259</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>10075</v>
       </c>
@@ -16769,36 +16699,36 @@
       <c r="C18" s="2" t="n">
         <v>43675.2926388889</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="n">
+      <c r="F18" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="7" t="n">
         <v>10268132</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="7" t="n">
         <v>2469848349</v>
       </c>
-      <c r="I18" s="4" t="n">
+      <c r="I18" s="7" t="n">
         <v>0.0810093801220133</v>
       </c>
-      <c r="J18" s="4" t="n">
+      <c r="J18" s="7" t="n">
         <v>20.1215207635646</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>10081</v>
       </c>
@@ -16808,36 +16738,36 @@
       <c r="C19" s="2" t="n">
         <v>43675.6711226852</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="n">
+      <c r="F19" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="n">
         <v>2677335</v>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="7" t="n">
         <v>2996604272</v>
       </c>
-      <c r="I19" s="4" t="n">
+      <c r="I19" s="7" t="n">
         <v>0.0099583257174447</v>
       </c>
-      <c r="J19" s="4" t="n">
+      <c r="J19" s="7" t="n">
         <v>24.1151198076123</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="20" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>10087</v>
       </c>
@@ -16847,36 +16777,36 @@
       <c r="C20" s="2" t="n">
         <v>43676.1033217593</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G20" s="4" t="n">
+      <c r="F20" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="n">
         <v>120585139</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="7" t="n">
         <v>3832870334</v>
       </c>
-      <c r="I20" s="4" t="n">
+      <c r="I20" s="7" t="n">
         <v>0.615124757946367</v>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="7" t="n">
         <v>28.272095138071</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>10159</v>
       </c>
@@ -16886,36 +16816,36 @@
       <c r="C21" s="2" t="n">
         <v>43680.7609837963</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G21" s="4" t="n">
+      <c r="F21" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="n">
         <v>13537185</v>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="7" t="n">
         <v>8800649415</v>
       </c>
-      <c r="I21" s="4" t="n">
+      <c r="I21" s="7" t="n">
         <v>0.124053069449311</v>
       </c>
-      <c r="J21" s="4" t="n">
+      <c r="J21" s="7" t="n">
         <v>53.6659925878956</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="10" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>10161</v>
       </c>
@@ -16925,32 +16855,32 @@
       <c r="C22" s="2" t="n">
         <v>43680.7929976852</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G22" s="4" t="n">
+      <c r="F22" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="n">
         <v>5874700</v>
       </c>
-      <c r="H22" s="4" t="n">
+      <c r="H22" s="7" t="n">
         <v>8806524115</v>
       </c>
-      <c r="I22" s="4" t="n">
+      <c r="I22" s="7" t="n">
         <v>0.0470269347393561</v>
       </c>
-      <c r="J22" s="4" t="n">
+      <c r="J22" s="7" t="n">
         <v>53.713019522635</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="10" t="s">
         <v>244</v>
       </c>
     </row>
@@ -16989,7 +16919,7 @@
       <c r="K23" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -17028,7 +16958,7 @@
       <c r="K24" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -17067,11 +16997,11 @@
       <c r="K25" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="26" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>10260</v>
       </c>
@@ -17081,36 +17011,36 @@
       <c r="C26" s="2" t="n">
         <v>43686.3598263889</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="4" t="n">
+      <c r="F26" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="n">
         <v>8909870</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="7" t="n">
         <v>11431769048</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="7" t="n">
         <v>0.0642901586568275</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="7" t="n">
         <v>73.6971300511074</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L26" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>10265</v>
       </c>
@@ -17120,36 +17050,36 @@
       <c r="C27" s="2" t="n">
         <v>43686.79625</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G27" s="4" t="n">
+      <c r="F27" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="n">
         <v>23314663</v>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="7" t="n">
         <v>12108562270</v>
       </c>
-      <c r="I27" s="4" t="n">
+      <c r="I27" s="7" t="n">
         <v>0.176059633740669</v>
       </c>
-      <c r="J27" s="4" t="n">
+      <c r="J27" s="7" t="n">
         <v>78.406345332215</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="L27" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="28" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>10270</v>
       </c>
@@ -17159,33 +17089,33 @@
       <c r="C28" s="2" t="n">
         <v>43687.3429166667</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G28" s="4" t="n">
+      <c r="F28" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="7" t="n">
         <v>7211481</v>
       </c>
-      <c r="H28" s="4" t="n">
+      <c r="H28" s="7" t="n">
         <v>13042905398</v>
       </c>
-      <c r="I28" s="4" t="n">
+      <c r="I28" s="7" t="n">
         <v>0.050721034761261</v>
       </c>
-      <c r="J28" s="4" t="n">
+      <c r="J28" s="7" t="n">
         <v>85.0670956307014</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="L28" s="3" t="s">
-        <v>247</v>
+      <c r="L28" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17223,8 +17153,8 @@
       <c r="K29" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="L29" s="3" t="s">
-        <v>248</v>
+      <c r="L29" s="6" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17262,11 +17192,11 @@
       <c r="K30" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="L30" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="31" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L30" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>10289</v>
       </c>
@@ -17276,36 +17206,36 @@
       <c r="C31" s="2" t="n">
         <v>43688.3976967593</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G31" s="4" t="n">
+      <c r="F31" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="n">
         <v>4276759</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="7" t="n">
         <v>14639972531</v>
       </c>
-      <c r="I31" s="4" t="n">
+      <c r="I31" s="7" t="n">
         <v>0.0305288644546685</v>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="7" t="n">
         <v>96.4453167384441</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="32" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L31" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>10297</v>
       </c>
@@ -17315,36 +17245,36 @@
       <c r="C32" s="2" t="n">
         <v>43688.6776388889</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G32" s="4" t="n">
+      <c r="F32" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="n">
         <v>5929141</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="7" t="n">
         <v>14916998658</v>
       </c>
-      <c r="I32" s="4" t="n">
+      <c r="I32" s="7" t="n">
         <v>0.044102279001774</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="7" t="n">
         <v>98.4221518311316</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L32" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="33" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L32" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>10299</v>
       </c>
@@ -17354,36 +17284,36 @@
       <c r="C33" s="2" t="n">
         <v>43688.7453819444</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G33" s="4" t="n">
+      <c r="F33" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G33" s="7" t="n">
         <v>101487282</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="7" t="n">
         <v>15045762692</v>
       </c>
-      <c r="I33" s="4" t="n">
+      <c r="I33" s="7" t="n">
         <v>0.725246592499597</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="7" t="n">
         <v>99.3430248668133</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="34" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L33" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>10316</v>
       </c>
@@ -17393,36 +17323,36 @@
       <c r="C34" s="2" t="n">
         <v>43689.3968634259</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G34" s="4" t="n">
+      <c r="F34" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="n">
         <v>3737095</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="7" t="n">
         <v>16184641036</v>
       </c>
-      <c r="I34" s="4" t="n">
+      <c r="I34" s="7" t="n">
         <v>0.0269581736182518</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="7" t="n">
         <v>107.435464888245</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L34" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="35" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L34" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>10321</v>
       </c>
@@ -17432,33 +17362,33 @@
       <c r="C35" s="2" t="n">
         <v>43689.6632291667</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="D35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G35" s="4" t="n">
+      <c r="F35" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="7" t="n">
         <v>8962220</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="7" t="n">
         <v>16687620707</v>
       </c>
-      <c r="I35" s="4" t="n">
+      <c r="I35" s="7" t="n">
         <v>0.0659972910769215</v>
       </c>
-      <c r="J35" s="4" t="n">
+      <c r="J35" s="7" t="n">
         <v>111.016144996974</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L35" s="3" t="s">
-        <v>253</v>
+      <c r="L35" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17496,7 +17426,7 @@
       <c r="K36" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -17535,8 +17465,8 @@
       <c r="K37" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L37" s="3" t="s">
-        <v>254</v>
+      <c r="L37" s="6" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17574,11 +17504,11 @@
       <c r="K38" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L38" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L38" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>10366</v>
       </c>
@@ -17588,36 +17518,36 @@
       <c r="C39" s="2" t="n">
         <v>43694.6866550926</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D39" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G39" s="4" t="n">
+      <c r="F39" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G39" s="7" t="n">
         <v>9318140</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="7" t="n">
         <v>17842323583</v>
       </c>
-      <c r="I39" s="4" t="n">
+      <c r="I39" s="7" t="n">
         <v>0.0318351812061231</v>
       </c>
-      <c r="J39" s="4" t="n">
+      <c r="J39" s="7" t="n">
         <v>119.011377238429</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L39" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="40" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>10369</v>
       </c>
@@ -17627,36 +17557,36 @@
       <c r="C40" s="2" t="n">
         <v>43694.7039814815</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="4" t="s">
+      <c r="D40" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F40" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G40" s="4" t="n">
+      <c r="F40" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G40" s="7" t="n">
         <v>4297641</v>
       </c>
-      <c r="H40" s="4" t="n">
+      <c r="H40" s="7" t="n">
         <v>17846621224</v>
       </c>
-      <c r="I40" s="4" t="n">
+      <c r="I40" s="7" t="n">
         <v>0.0148379990469577</v>
       </c>
-      <c r="J40" s="4" t="n">
+      <c r="J40" s="7" t="n">
         <v>119.026215237476</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>10407</v>
       </c>
@@ -17666,33 +17596,33 @@
       <c r="C41" s="2" t="n">
         <v>43696.7258217593</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="D41" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="F41" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G41" s="4" t="n">
+      <c r="F41" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="7" t="n">
         <v>5553789</v>
       </c>
-      <c r="H41" s="4" t="n">
+      <c r="H41" s="7" t="n">
         <v>21325918002</v>
       </c>
-      <c r="I41" s="4" t="n">
+      <c r="I41" s="7" t="n">
         <v>0.022664580593315</v>
       </c>
-      <c r="J41" s="4" t="n">
+      <c r="J41" s="7" t="n">
         <v>130.971590880116</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L41" s="3" t="s">
-        <v>253</v>
+      <c r="L41" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17730,8 +17660,8 @@
       <c r="K42" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="L42" s="7" t="s">
-        <v>255</v>
+      <c r="L42" s="10" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17769,7 +17699,7 @@
       <c r="K43" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -17808,8 +17738,8 @@
       <c r="K44" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="L44" s="7" t="s">
-        <v>256</v>
+      <c r="L44" s="10" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17847,8 +17777,8 @@
       <c r="K45" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>257</v>
+      <c r="L45" s="10" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17886,8 +17816,8 @@
       <c r="K46" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="7" t="s">
-        <v>256</v>
+      <c r="L46" s="10" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17925,11 +17855,11 @@
       <c r="K47" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="L47" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>10463</v>
       </c>
@@ -17939,36 +17869,36 @@
       <c r="C48" s="2" t="n">
         <v>43701.8556828704</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F48" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G48" s="4" t="n">
+      <c r="F48" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="7" t="n">
         <v>11539139</v>
       </c>
-      <c r="H48" s="4" t="n">
+      <c r="H48" s="7" t="n">
         <v>25183842753</v>
       </c>
-      <c r="I48" s="4" t="n">
+      <c r="I48" s="7" t="n">
         <v>0.0442569562327692</v>
       </c>
-      <c r="J48" s="4" t="n">
+      <c r="J48" s="7" t="n">
         <v>147.019631841557</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="L48" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="49" s="4" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" s="7" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>10485</v>
       </c>
@@ -17978,33 +17908,33 @@
       <c r="C49" s="2" t="n">
         <v>43702.365</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="D49" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F49" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G49" s="4" t="n">
+      <c r="F49" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="7" t="n">
         <v>1646586</v>
       </c>
-      <c r="H49" s="4" t="n">
+      <c r="H49" s="7" t="n">
         <v>25834990054</v>
       </c>
-      <c r="I49" s="4" t="n">
+      <c r="I49" s="7" t="n">
         <v>0.00627976754987283</v>
       </c>
-      <c r="J49" s="4" t="n">
+      <c r="J49" s="7" t="n">
         <v>149.279656989349</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K49" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>258</v>
+      <c r="L49" s="8" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18042,7 +17972,7 @@
       <c r="K50" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="L50" s="3" t="s">
+      <c r="L50" s="6" t="s">
         <v>145</v>
       </c>
     </row>
@@ -18081,11 +18011,11 @@
       <c r="K51" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="L51" s="3" t="s">
+      <c r="L51" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="52" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>10544</v>
       </c>
@@ -18095,36 +18025,36 @@
       <c r="C52" s="2" t="n">
         <v>43705.7600115741</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="D52" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F52" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G52" s="4" t="n">
+      <c r="F52" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="7" t="n">
         <v>2781103</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="7" t="n">
         <v>30724480615</v>
       </c>
-      <c r="I52" s="4" t="n">
+      <c r="I52" s="7" t="n">
         <v>0.0101925026622066</v>
       </c>
-      <c r="J52" s="4" t="n">
+      <c r="J52" s="7" t="n">
         <v>181.037556707155</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K52" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="L52" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="53" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L52" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>10550</v>
       </c>
@@ -18134,36 +18064,36 @@
       <c r="C53" s="2" t="n">
         <v>43706.2142939815</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E53" s="4" t="s">
+      <c r="D53" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F53" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G53" s="4" t="n">
+      <c r="F53" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G53" s="7" t="n">
         <v>6097423</v>
       </c>
-      <c r="H53" s="4" t="n">
+      <c r="H53" s="7" t="n">
         <v>31611545258</v>
       </c>
-      <c r="I53" s="4" t="n">
+      <c r="I53" s="7" t="n">
         <v>0.0233472944309801</v>
       </c>
-      <c r="J53" s="4" t="n">
+      <c r="J53" s="7" t="n">
         <v>184.371406523456</v>
       </c>
-      <c r="K53" s="4" t="s">
+      <c r="K53" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="54" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L53" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>10569</v>
       </c>
@@ -18173,36 +18103,36 @@
       <c r="C54" s="2" t="n">
         <v>43706.8109259259</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E54" s="4" t="s">
+      <c r="D54" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F54" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G54" s="4" t="n">
+      <c r="F54" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G54" s="7" t="n">
         <v>1421075</v>
       </c>
-      <c r="H54" s="4" t="n">
+      <c r="H54" s="7" t="n">
         <v>32574090556</v>
       </c>
-      <c r="I54" s="4" t="n">
+      <c r="I54" s="7" t="n">
         <v>0.0053261071957413</v>
       </c>
-      <c r="J54" s="4" t="n">
+      <c r="J54" s="7" t="n">
         <v>187.994408302</v>
       </c>
-      <c r="K54" s="4" t="s">
+      <c r="K54" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="L54" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="55" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L54" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>10572</v>
       </c>
@@ -18212,36 +18142,36 @@
       <c r="C55" s="2" t="n">
         <v>43707.1466666667</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="D55" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F55" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G55" s="4" t="n">
+      <c r="F55" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G55" s="7" t="n">
         <v>5635763</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="7" t="n">
         <v>33292933105</v>
       </c>
-      <c r="I55" s="4" t="n">
+      <c r="I55" s="7" t="n">
         <v>0.0211575231192647</v>
       </c>
-      <c r="J55" s="4" t="n">
+      <c r="J55" s="7" t="n">
         <v>190.682182289446</v>
       </c>
-      <c r="K55" s="4" t="s">
+      <c r="K55" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="L55" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="56" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L55" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56" s="7" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>10573</v>
       </c>
@@ -18251,36 +18181,36 @@
       <c r="C56" s="2" t="n">
         <v>43707.1588425926</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="D56" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F56" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G56" s="4" t="n">
+      <c r="F56" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G56" s="7" t="n">
         <v>21146533</v>
       </c>
-      <c r="H56" s="4" t="n">
+      <c r="H56" s="7" t="n">
         <v>33314079638</v>
       </c>
-      <c r="I56" s="4" t="n">
+      <c r="I56" s="7" t="n">
         <v>0.0789706949557805</v>
       </c>
-      <c r="J56" s="4" t="n">
+      <c r="J56" s="7" t="n">
         <v>190.761152984402</v>
       </c>
-      <c r="K56" s="4" t="s">
+      <c r="K56" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="L56" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="57" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>10579</v>
       </c>
@@ -18290,36 +18220,36 @@
       <c r="C57" s="2" t="n">
         <v>43707.5736805556</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="D57" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F57" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G57" s="4" t="n">
+      <c r="F57" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G57" s="7" t="n">
         <v>2714734</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="7" t="n">
         <v>33731858312</v>
       </c>
-      <c r="I57" s="4" t="n">
+      <c r="I57" s="7" t="n">
         <v>0.0102044242688217</v>
       </c>
-      <c r="J57" s="4" t="n">
+      <c r="J57" s="7" t="n">
         <v>192.329521405127</v>
       </c>
-      <c r="K57" s="4" t="s">
+      <c r="K57" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="L57" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L57" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>10582</v>
       </c>
@@ -18329,33 +18259,33 @@
       <c r="C58" s="2" t="n">
         <v>43707.5959490741</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="D58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F58" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G58" s="4" t="n">
+      <c r="F58" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G58" s="7" t="n">
         <v>13869136</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="7" t="n">
         <v>33745727448</v>
       </c>
-      <c r="I58" s="4" t="n">
+      <c r="I58" s="7" t="n">
         <v>0.0525149583058122</v>
       </c>
-      <c r="J58" s="4" t="n">
+      <c r="J58" s="7" t="n">
         <v>192.382036363432</v>
       </c>
-      <c r="K58" s="4" t="s">
+      <c r="K58" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="L58" s="5" t="s">
-        <v>263</v>
+      <c r="L58" s="8" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18392,8 +18322,8 @@
       <c r="K59" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="L59" s="5" t="s">
-        <v>264</v>
+      <c r="L59" s="8" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18430,8 +18360,8 @@
       <c r="K60" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="L60" s="5" t="s">
-        <v>265</v>
+      <c r="L60" s="8" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18468,8 +18398,8 @@
       <c r="K61" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="L61" s="5" t="s">
-        <v>266</v>
+      <c r="L61" s="8" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18507,7 +18437,7 @@
       <c r="K62" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="L62" s="3" t="s">
+      <c r="L62" s="6" t="s">
         <v>208</v>
       </c>
     </row>
@@ -18546,7 +18476,7 @@
       <c r="K63" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="L63" s="3" t="s">
+      <c r="L63" s="6" t="s">
         <v>208</v>
       </c>
     </row>
@@ -18585,7 +18515,7 @@
       <c r="K64" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="L64" s="3" t="s">
+      <c r="L64" s="6" t="s">
         <v>208</v>
       </c>
     </row>
@@ -18624,8 +18554,8 @@
       <c r="K65" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="L65" s="7" t="s">
-        <v>267</v>
+      <c r="L65" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18663,11 +18593,11 @@
       <c r="K66" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="L66" s="3" t="s">
+      <c r="L66" s="6" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="67" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>10680</v>
       </c>
@@ -18677,36 +18607,36 @@
       <c r="C67" s="2" t="n">
         <v>43713.2175231482</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E67" s="4" t="s">
+      <c r="D67" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E67" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="F67" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G67" s="4" t="n">
+      <c r="F67" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G67" s="7" t="n">
         <v>7585438</v>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H67" s="7" t="n">
         <v>41056141689</v>
       </c>
-      <c r="I67" s="4" t="n">
+      <c r="I67" s="7" t="n">
         <v>0.034537353127544</v>
       </c>
-      <c r="J67" s="4" t="n">
+      <c r="J67" s="7" t="n">
         <v>224.569074047073</v>
       </c>
-      <c r="K67" s="4" t="s">
+      <c r="K67" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="L67" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="68" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="7" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>10703</v>
       </c>
@@ -18716,36 +18646,36 @@
       <c r="C68" s="2" t="n">
         <v>43715.231712963</v>
       </c>
-      <c r="D68" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E68" s="4" t="s">
+      <c r="D68" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="F68" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G68" s="4" t="n">
+      <c r="F68" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G68" s="7" t="n">
         <v>2415976</v>
       </c>
-      <c r="H68" s="4" t="n">
+      <c r="H68" s="7" t="n">
         <v>43336656862</v>
       </c>
-      <c r="I68" s="4" t="n">
+      <c r="I68" s="7" t="n">
         <v>0.0111393578258425</v>
       </c>
-      <c r="J68" s="4" t="n">
+      <c r="J68" s="7" t="n">
         <v>236.131865254245</v>
       </c>
-      <c r="K68" s="4" t="s">
+      <c r="K68" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="L68" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="69" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L68" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <v>10727</v>
       </c>
@@ -18755,32 +18685,32 @@
       <c r="C69" s="2" t="n">
         <v>43716.511400463</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E69" s="4" t="s">
+      <c r="D69" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="F69" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G69" s="4" t="n">
+      <c r="F69" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G69" s="7" t="n">
         <v>6299373</v>
       </c>
-      <c r="H69" s="4" t="n">
+      <c r="H69" s="7" t="n">
         <v>44829291404</v>
       </c>
-      <c r="I69" s="4" t="n">
+      <c r="I69" s="7" t="n">
         <v>0.0293794996478341</v>
       </c>
-      <c r="J69" s="4" t="n">
+      <c r="J69" s="7" t="n">
         <v>243.945001008463</v>
       </c>
-      <c r="K69" s="4" t="s">
+      <c r="K69" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="L69" s="3" t="s">
+      <c r="L69" s="6" t="s">
         <v>208</v>
       </c>
     </row>
@@ -18802,8 +18732,8 @@
   </sheetPr>
   <dimension ref="A17:L18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="1" sqref="249:289 L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18853,8 +18783,8 @@
       <c r="K17" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>269</v>
+      <c r="L17" s="8" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18892,8 +18822,8 @@
       <c r="K18" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>269</v>
+      <c r="L18" s="8" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added another sheet representing the list of Hodo Calibration Runs
</commit_message>
<xml_diff>
--- a/RunTableAdditions.xlsx
+++ b/RunTableAdditions.xlsx
@@ -12,7 +12,7 @@
     <sheet name="MissinginMaurik" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="MissingCameron" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="SpecialAttention" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HodoCalibRuns" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1279,8 +1279,8 @@
   </sheetPr>
   <dimension ref="A1:O422"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20741,8 +20741,8 @@
   </sheetPr>
   <dimension ref="A7:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21121,7 +21121,7 @@
   </sheetPr>
   <dimension ref="A14:L69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -23452,16 +23452,18 @@
   </sheetPr>
   <dimension ref="C17:G54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K31" activeCellId="0" sqref="K31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
the RunTableAdditions.xlsx was modified
</commit_message>
<xml_diff>
--- a/RunTableAdditions.xlsx
+++ b/RunTableAdditions.xlsx
@@ -1279,8 +1279,8 @@
   </sheetPr>
   <dimension ref="A1:O422"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A267" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A280" activeCellId="0" sqref="A280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23452,8 +23452,8 @@
   </sheetPr>
   <dimension ref="C17:G54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P35" activeCellId="0" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23961,7 +23961,7 @@
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="13" t="n">
-        <v>10524</v>
+        <v>10525</v>
       </c>
       <c r="D46" s="13" t="n">
         <v>10535</v>

</xml_diff>